<commit_message>
OpenPyXL: Copy Range: Translate Long Column to Form
</commit_message>
<xml_diff>
--- a/python/openpyxl/copy-range/data.xlsx
+++ b/python/openpyxl/copy-range/data.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="92">
   <si>
     <t xml:space="preserve">Output Tax Invoice</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">Approval Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Month Period</t>
+    <t xml:space="preserve">Period</t>
   </si>
   <si>
     <t xml:space="preserve">Base Price</t>
@@ -73,13 +73,13 @@
     <t xml:space="preserve">VAT</t>
   </si>
   <si>
-    <t xml:space="preserve">Tanggal Rekam</t>
+    <t xml:space="preserve">Record Date</t>
   </si>
   <si>
     <t xml:space="preserve">VAT Lux</t>
   </si>
   <si>
-    <t xml:space="preserve">Record Date</t>
+    <t xml:space="preserve">Record User</t>
   </si>
   <si>
     <t xml:space="preserve">Tax Inv Status</t>
@@ -252,9 +252,6 @@
   </si>
   <si>
     <t xml:space="preserve">Approval Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Record User</t>
   </si>
   <si>
     <t xml:space="preserve">Earth Wind And Flour, Ltd</t>
@@ -818,9 +815,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>547920</xdr:colOff>
+      <xdr:colOff>546480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>317880</xdr:rowOff>
+      <xdr:rowOff>316440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -834,7 +831,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="360000" y="190800"/>
-          <a:ext cx="5392440" cy="1079640"/>
+          <a:ext cx="5391000" cy="1078200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -860,9 +857,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>547920</xdr:colOff>
+      <xdr:colOff>546480</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>317880</xdr:rowOff>
+      <xdr:rowOff>316440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -876,7 +873,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="360000" y="190800"/>
-          <a:ext cx="5392440" cy="1079640"/>
+          <a:ext cx="5391000" cy="1078200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -912,8 +909,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="16.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="4.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="4.09"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="15" min="14" style="2" width="21.43"/>
@@ -1381,7 +1378,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="13.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="4.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="4.09"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1734,7 +1731,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="2" width="21.43"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="2" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="2" width="13.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="4.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="4.09"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1853,10 +1850,10 @@
         <v>7</v>
       </c>
       <c r="Q6" s="45" t="s">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="R6" s="45" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="S6" s="45" t="s">
         <v>20</v>
@@ -1870,7 +1867,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" s="49" t="s">
         <v>43</v>
@@ -1879,7 +1876,7 @@
         <v>44</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="50" t="n">
         <v>1</v>
@@ -1900,28 +1897,28 @@
         <v>0</v>
       </c>
       <c r="L7" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="M7" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="M7" s="49" t="s">
+      <c r="N7" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="N7" s="50" t="s">
+      <c r="O7" s="50" t="s">
         <v>79</v>
-      </c>
-      <c r="O7" s="50" t="s">
-        <v>80</v>
       </c>
       <c r="P7" s="49" t="s">
         <v>51</v>
       </c>
       <c r="Q7" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="R7" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="R7" s="49" t="s">
-        <v>81</v>
-      </c>
       <c r="S7" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T7" s="49"/>
     </row>
@@ -1930,7 +1927,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" s="49" t="s">
         <v>54</v>
@@ -1939,7 +1936,7 @@
         <v>55</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="50" t="n">
         <v>1</v>
@@ -1948,7 +1945,7 @@
         <v>2022</v>
       </c>
       <c r="H8" s="50" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I8" s="51" t="n">
         <v>13000000</v>
@@ -1960,28 +1957,28 @@
         <v>0</v>
       </c>
       <c r="L8" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M8" s="49" t="s">
+        <v>84</v>
+      </c>
+      <c r="N8" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="N8" s="50" t="s">
+      <c r="O8" s="50" t="s">
         <v>86</v>
-      </c>
-      <c r="O8" s="50" t="s">
-        <v>87</v>
       </c>
       <c r="P8" s="49" t="s">
         <v>61</v>
       </c>
       <c r="Q8" s="50" t="s">
+        <v>86</v>
+      </c>
+      <c r="R8" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="R8" s="49" t="s">
-        <v>88</v>
-      </c>
       <c r="S8" s="50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T8" s="49"/>
     </row>
@@ -1990,7 +1987,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="49" t="s">
         <v>64</v>
@@ -1999,7 +1996,7 @@
         <v>65</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F9" s="50" t="n">
         <v>1</v>
@@ -2020,28 +2017,28 @@
         <v>0</v>
       </c>
       <c r="L9" s="50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M9" s="49" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="N9" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="O9" s="50" t="s">
         <v>79</v>
-      </c>
-      <c r="O9" s="50" t="s">
-        <v>80</v>
       </c>
       <c r="P9" s="49" t="s">
         <v>68</v>
       </c>
       <c r="Q9" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R9" s="49" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S9" s="50" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T9" s="49"/>
     </row>

</xml_diff>